<commit_message>
@Guss00 Atualização do Chat
</commit_message>
<xml_diff>
--- a/Mercurio/Documentacao/PlanilhaDeRiscoMercurio.xlsx
+++ b/Mercurio/Documentacao/PlanilhaDeRiscoMercurio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felip\OneDrive\Área de Trabalho\PO Sprint 2 C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eef80a03af613308/Área de Trabalho/Clone/Sprint2/Mercurio/Documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AAEE36B-084B-46CA-B2BF-3820B62039A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{7AAEE36B-084B-46CA-B2BF-3820B62039A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FBA363F-A003-4AA9-94B3-03E5BF6CA6EC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -350,11 +350,94 @@
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -364,110 +447,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,41 +747,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="77" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="24" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="32.7109375" customWidth="1"/>
+    <col min="9" max="24" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -800,14 +800,14 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -826,22 +826,22 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="1"/>
@@ -862,14 +862,14 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -888,304 +888,304 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A7" s="2">
+      <c r="A7" s="35">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="37">
         <v>1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="37">
         <v>3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="43">
         <v>3</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="43"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="44"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A10" s="2">
+      <c r="A10" s="35">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="37">
         <v>2</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="37">
         <v>2</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="43">
         <v>4</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="43"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="44"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:24" ht="39.75" customHeight="1">
-      <c r="A13" s="2">
+      <c r="A13" s="35">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="46">
         <v>1</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="46">
         <v>3</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="46">
         <v>3</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="39.75" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="44"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A15" s="2">
+      <c r="A15" s="35">
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="37">
         <v>1</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="37">
         <v>3</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="43">
         <v>3</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="24.75" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="45"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="46"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="51"/>
     </row>
     <row r="18" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A18" s="2">
+      <c r="A18" s="35">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="37">
         <v>2</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="37">
         <v>3</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="43">
         <v>6</v>
       </c>
       <c r="F18" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="53"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="15"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="53"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="16"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="54"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="44"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A22" s="2">
+      <c r="A22" s="35">
         <v>6</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="37">
         <v>1</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="37">
         <v>3</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="43">
         <v>3</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="43"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" ht="24.75" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="44"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="24.75" customHeight="1"/>
     <row r="26" spans="1:8" ht="24.75" customHeight="1"/>
@@ -2165,35 +2165,25 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="F1:F6"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="C1:E2"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="F22:F24"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B13:B14"/>
@@ -2206,25 +2196,35 @@
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="F1:F6"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="F7:F9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>